<commit_message>
some edit and delete
</commit_message>
<xml_diff>
--- a/papers_list.xlsx
+++ b/papers_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\86188\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\自动化测试\automated-testing-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00B1FD5A-8604-4DC1-B11B-C2831CAE44CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF1DF65-CD6D-458A-A418-B4F01C01839C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>title</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,6 +55,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Applying Mutation Testing to Web Applications</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>U. Praphamontripong and J. Offutt, "Applying Mutation Testing to Web Applications," 2010 Third International Conference on Software Testing, Verification, and Validation Workshops, 2010, pp. 132-141, doi: 10.1109/ICSTW.2010.38.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Rudolf Ramler, Thomas Wetzlmaier, and Claus Klammer. 2017. An empirical study on the application of mutation testing for a safety-critical industrial software system. In Proceedings of the Symposium on Applied Computing (SAC '17). Association for Computing Machinery, New York, NY, USA, 1401–1408.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -63,6 +71,14 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>De Souza S D R S, Maldonado J C, Fabbri S C P F, et al. Mutation testing applied to estelle specifications[J]. Software Quality Journal, 1999, 8(4): 285-301.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mutation Testing Applied to Estelle Specifications</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Betka M, Wagner S. Towards practical application of mutation testing in industry—Traditional versus extreme mutation testing[J]. Journal of Software: Evolution and Process, 2022: e2450.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -71,9 +87,25 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Applying Mutation Testing to XML Schemas</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Franzotte L, Vergilio S R. Applying Mutation Testing in XML Schemas[C]//SEKE. 2006: 511-516.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mutation Testing Applied to Hardware: the Mutants Generation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>MDroid+: A Mutation Testing Framework for Android</t>
   </si>
   <si>
+    <t>Nguyen T B, Robach C. Mutation testing applied to hardware: the mutants generation[C]//Proceedings of the 11th IFIP International Conference on Very Large Scale Integration. 2001: 118-123.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Moran K, Tufano M, Bernal-Cárdenas C, et al. Mdroid+: A mutation testing framework for android[C]//2018 IEEE/ACM 40th International Conference on Software Engineering: Companion (ICSE-Companion). IEEE, 2018: 33-36.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,50 +155,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Lei Ma, Fuyuan Zhang, Jiyuan Sun, Minhui Xue, Bo Li, Felix Juefei-Xu DeepMutation: Mutation Testing of Deep Learning Systems</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M.R.Woodward and K.Halewood Department of Computer Science, University of Liverpool,P.O. Box 147, Liverpool, L69 3BX, U.K.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FROM WEAK TO STRONG, DEAD OR ALIVE?AN ANALYSIS OF SOME MUTATION TESTING ISSUES.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>An Empirical Evaluation of the First and Second Order Mutation Testing Strategies</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mike Papadakis and Nicos Malevris Department of Informatics, Athens University of Economics and Business</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Athens, Greece</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reducing the Cost of Mutation Testing:An Empirical Study</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W. Eric Wong Bell Communications Research, Morristown, New Jersey Aditya P. Mathur Department of Computer Sciences, Purdue University, West Lafayette, Indiana Reducing the Cost of Mutation Testing:An Empirical Study</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Weak Mutation Testing and Completeness of Test Sets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">WILLIAM E. HOWDEN </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IEEE TRANSACTIONS ON SOFTWARE ENGINEERING, VOL. SE-8, NO. 4, JULY 1982</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> SSDI 0164.1212(94)00098-8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -179,52 +167,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2018 IEEE 29th International Symposium on Software Reliability Engineering</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Alessandro Viola Pizzoleto, Fabiano Cutigi Ferrari, Jeff Offutt, Leo Fernandes,Márcio Ribeiro A systematic literature review of techniques and metrics to reduce the cost of mutation testing  </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The Journal of Systems and Software 157 (2019) 110388</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CODE DEFENDERS: A Mutation Testing Game</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Jose Miguel Rojas, Gordon Fraser Department of Computer Science, The University of Sheffield, Sheffield, United Kingdom CODE DEFENDERS: A Mutation Testing Game：eprints.whiterose.ac.uk/116454/1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Mutation testing applied to validate specifications based on Petri Nets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S.C.P.F. FabbriO J. C. Maldonado P.C.Masiero ME.Delamaro E. Wong</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> Mutation testing applied to validate specifications based on Petri Nets</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>link.springer.com/content/pdf/10.1007/978-0-387-34945-9_24</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Metallaxis‐FL: mutation‐based fault localization</t>
   </si>
   <si>
@@ -243,28 +189,56 @@
     <t>Papadakis M, Le Traon Y. Effective fault localization via mutation analysis: A selective mutation approach[C]//Proceedings of the 29th annual ACM symposium on applied computing. 2014: 1293-1300.</t>
   </si>
   <si>
-    <t>Adversarial Sample Detection for Deep Neural Network through Model Mutation Testing</t>
+    <t>Pizzoleto A V, Ferrari F C, Offutt J, et al. A systematic literature review of techniques and metrics to reduce the cost of mutation testing[J]. Journal of Systems and Software, 2019, 157: 110388.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ma L, Zhang F, Sun J, et al. Deepmutation: Mutation testing of deep learning systems[C]//2018 IEEE 29th International Symposium on Software Reliability Engineering (ISSRE). IEEE, 2018: 100-111.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rojas J M, Fraser G. Code defenders: a mutation testing game[C]//2016 IEEE Ninth International Conference on Software Testing, Verification and Validation Workshops (ICSTW). IEEE, 2016: 162-167.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Adversarial sample detection for deep neural network through model mutation testing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Wang J, Dong G, Sun J, et al. Adversarial sample detection for deep neural network through model mutation testing[C]//2019 IEEE/ACM 41st International Conference on Software Engineering (ICSE). IEEE, 2019: 1245-1256.</t>
-  </si>
-  <si>
-    <t>Mitigating the Effects of Flaky Tests on Mutation Testing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mitigating the effects of flaky tests on mutation testing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Shi A, Bell J, Marinov D. Mitigating the effects of flaky tests on mutation testing[C]//Proceedings of the 28th ACM SIGSOFT International Symposium on Software Testing and Analysis. 2019: 112-122.</t>
-  </si>
-  <si>
-    <t>Assessing Test Case Prioritization on Real Faults and Mutants</t>
-  </si>
-  <si>
-    <t>Luo Q, Moran K, Poshyvanyk D, et al. Assessing test case prioritization on real faults and mutants[C]//2018 IEEE international conference on software maintenance and evolution (ICSME). IEEE, 2018: 240-251.</t>
-  </si>
-  <si>
-    <t>Empirical Evaluation of Mutation-based Test Case Prioritization Techniques</t>
-  </si>
-  <si>
-    <t>Shin D, Yoo S, Papadakis M, et al. Empirical evaluation of mutation‐based test case prioritization techniques[J]. Software Testing, Verification and Reliability, 2019, 29(1-2): e1695.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>An extensive study on cross-project predictive mutation testing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mao D, Chen L, Zhang L. An extensive study on cross-project predictive mutation testing[C]//2019 12th IEEE Conference on Software Testing, Validation and Verification (ICST). IEEE, 2019: 160-171.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Wodel-Test: a model-based framework for language-independent mutation testing</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gómez-Abajo P, Guerra E, Lara J, et al. Wodel-Test: a model-based framework for language-independent mutation testing[J]. Software and Systems Modeling, 2021, 20(3): 767-793.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Evolutionary mutation testing for IoT with recorded and generated events</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gutiérrez‐Madroñal L, García‐Domínguez A, Medina‐Bulo I. Evolutionary mutation testing for IoT with recorded and generated events[J]. Software: Practice and Experience, 2019, 49(4): 640-672.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -289,22 +263,27 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="等线"/>
-      <family val="3"/>
+      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -312,18 +291,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="检查单元格" xfId="1" builtinId="23"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -601,19 +604,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V28"/>
+  <dimension ref="A1:BA28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="95.44140625" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="95.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -621,7 +623,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -629,7 +631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -637,7 +639,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -645,232 +647,263 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="1:53" ht="15" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="4"/>
+      <c r="X18" s="4"/>
+      <c r="Y18" s="4"/>
+      <c r="Z18" s="4"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="4"/>
+      <c r="AC18" s="4"/>
+      <c r="AD18" s="4"/>
+      <c r="AE18" s="4"/>
+      <c r="AF18" s="4"/>
+      <c r="AG18" s="4"/>
+      <c r="AH18" s="4"/>
+      <c r="AI18" s="4"/>
+      <c r="AJ18" s="4"/>
+      <c r="AK18" s="4"/>
+      <c r="AL18" s="4"/>
+      <c r="AM18" s="4"/>
+      <c r="AN18" s="4"/>
+      <c r="AO18" s="4"/>
+      <c r="AP18" s="4"/>
+      <c r="AQ18" s="4"/>
+      <c r="AR18" s="4"/>
+      <c r="AS18" s="4"/>
+      <c r="AT18" s="4"/>
+      <c r="AU18" s="4"/>
+      <c r="AV18" s="4"/>
+      <c r="AW18" s="4"/>
+      <c r="AX18" s="4"/>
+      <c r="AY18" s="4"/>
+      <c r="AZ18" s="4"/>
+      <c r="BA18" s="4"/>
+    </row>
+    <row r="19" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="V20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="T21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="V22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" t="s">
         <v>56</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="24" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B25" t="s">
         <v>58</v>
       </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
+    </row>
+    <row r="26" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="N19" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="M20" t="s">
-        <v>30</v>
-      </c>
-      <c r="V20" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="K21" t="s">
-        <v>33</v>
-      </c>
-      <c r="L21" t="s">
-        <v>31</v>
-      </c>
-      <c r="T21" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" t="s">
-        <v>35</v>
-      </c>
-      <c r="V22" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" t="s">
-        <v>36</v>
-      </c>
-      <c r="I23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="28" spans="1:53" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>44</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B28" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B25" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" t="s">
-        <v>48</v>
-      </c>
-      <c r="O25" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" t="s">
-        <v>55</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B18:BA18"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>